<commit_message>
wrote the function to calculate dpi
</commit_message>
<xml_diff>
--- a/data/AV_cohort_info.xlsx
+++ b/data/AV_cohort_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewding/Desktop/Projects/2024 CSF1R w:Dr. Kim/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7756338D-03B1-4041-B5B2-7AA523EA4FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23F306E-45B1-7049-AD2E-48DD72F76A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{0D63C5D4-A581-774F-AB15-A4F734F39EFF}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15140" xr2:uid="{0D63C5D4-A581-774F-AB15-A4F734F39EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="115">
   <si>
     <t>Animal_ID</t>
   </si>
@@ -841,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1556DF15-3C73-494E-A779-A5E23B23C9C6}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1447,57 +1447,99 @@
       <c r="G13" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="H13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>46261</v>
+        <v>42930</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>44</v>
+        <v>73</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>30</v>
+      </c>
+      <c r="R14" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>59</v>
+        <v>79</v>
+      </c>
+      <c r="U14" s="2">
+        <v>7.87</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>42930</v>
+        <v>44136</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -1539,89 +1581,63 @@
         <v>76</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="Q15" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="R15" s="1">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>78</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="U15" s="2">
-        <v>7.87</v>
+        <v>6.04</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44136</v>
+        <v>42537</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>33</v>
-      </c>
-      <c r="R16" s="1">
-        <v>4.7</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
       <c r="T16" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="U16" s="2">
-        <v>6.04</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="U16" s="2"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>42537</v>
+        <v>41543</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
@@ -1651,49 +1667,75 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>41543</v>
+        <v>44462</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="I18" s="2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>33</v>
+      </c>
+      <c r="R18" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="T18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="U18" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="U18" s="2">
+        <v>6.15</v>
+      </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44462</v>
+        <v>45060</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
@@ -1735,89 +1777,89 @@
         <v>96</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Q19" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R19" s="1">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>78</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="U19" s="2">
-        <v>6.15</v>
+        <v>5.21</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>45060</v>
+        <v>43205</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>68</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="Q20" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="R20" s="1">
-        <v>4.3</v>
+        <v>5.7</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="U20" s="2">
-        <v>5.21</v>
+        <v>8.07</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>43205</v>
+        <v>44653</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>15</v>
@@ -1835,7 +1877,7 @@
         <v>68</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>104</v>
@@ -1859,83 +1901,21 @@
         <v>109</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Q21" s="1">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="R21" s="1">
-        <v>5.7</v>
+        <v>5.3</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>78</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="U21" s="2">
-        <v>8.07</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>44653</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>37</v>
-      </c>
-      <c r="R22" s="1">
-        <v>5.3</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="U22" s="2">
         <v>6.86</v>
       </c>
     </row>

</xml_diff>